<commit_message>
Amélioration gestion de fichiers
Ajout icon, CodeBook.pdf
Amélioration gestion des fichiers
</commit_message>
<xml_diff>
--- a/CodeDesLivres.xlsx
+++ b/CodeDesLivres.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C9104C-E560-4CB3-A00A-D578F77BE1DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A7829AD-2A11-4D0F-BBF4-D62B30297583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-105" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -324,7 +324,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -399,11 +399,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -453,6 +468,28 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -791,10 +828,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D28"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38:D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -803,9 +843,10 @@
     <col min="2" max="2" width="52" customWidth="1"/>
     <col min="3" max="3" width="47" customWidth="1"/>
     <col min="4" max="4" width="32" customWidth="1"/>
+    <col min="5" max="5" width="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>2</v>
       </c>
@@ -818,9 +859,11 @@
       <c r="D1" s="12" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="3" t="s">
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+    </row>
+    <row r="2" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="17" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -832,9 +875,11 @@
       <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="3" t="s">
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+    </row>
+    <row r="3" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="17" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -846,9 +891,11 @@
       <c r="D3" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="1" t="s">
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+    </row>
+    <row r="4" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="18" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -860,9 +907,11 @@
       <c r="D4" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="3" t="s">
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+    </row>
+    <row r="5" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="17" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -874,9 +923,11 @@
       <c r="D5" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="5" t="s">
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+    </row>
+    <row r="6" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="19" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="6" t="s">
@@ -888,9 +939,11 @@
       <c r="D6" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="7" t="s">
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+    </row>
+    <row r="7" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="9" t="s">
@@ -902,9 +955,11 @@
       <c r="D7" s="7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="1" t="s">
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+    </row>
+    <row r="8" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="18" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -916,9 +971,11 @@
       <c r="D8" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="5" t="s">
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+    </row>
+    <row r="9" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="19" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="6" t="s">
@@ -930,9 +987,11 @@
       <c r="D9" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="5" t="s">
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+    </row>
+    <row r="10" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="19" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="6" t="s">
@@ -944,9 +1003,11 @@
       <c r="D10" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="7" t="s">
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+    </row>
+    <row r="11" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -958,9 +1019,11 @@
       <c r="D11" s="7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="7" t="s">
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+    </row>
+    <row r="12" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="20" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="9" t="s">
@@ -972,9 +1035,11 @@
       <c r="D12" s="7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="5" t="s">
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+    </row>
+    <row r="13" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="19" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="6" t="s">
@@ -986,9 +1051,11 @@
       <c r="D13" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="5" t="s">
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+    </row>
+    <row r="14" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="19" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="6" t="s">
@@ -1000,9 +1067,11 @@
       <c r="D14" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="3" t="s">
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+    </row>
+    <row r="15" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="17" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -1014,9 +1083,11 @@
       <c r="D15" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="7" t="s">
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+    </row>
+    <row r="16" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="20" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="9" t="s">
@@ -1028,9 +1099,11 @@
       <c r="D16" s="7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="7" t="s">
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+    </row>
+    <row r="17" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="20" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="9" t="s">
@@ -1042,9 +1115,11 @@
       <c r="D17" s="7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="3" t="s">
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+    </row>
+    <row r="18" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="4" t="s">
@@ -1056,9 +1131,11 @@
       <c r="D18" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="5" t="s">
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+    </row>
+    <row r="19" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="19" t="s">
         <v>20</v>
       </c>
       <c r="B19" s="6" t="s">
@@ -1070,9 +1147,11 @@
       <c r="D19" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="7" t="s">
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+    </row>
+    <row r="20" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="20" t="s">
         <v>25</v>
       </c>
       <c r="B20" s="9" t="s">
@@ -1084,9 +1163,11 @@
       <c r="D20" s="7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="5" t="s">
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+    </row>
+    <row r="21" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="19" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="14" t="s">
@@ -1098,9 +1179,11 @@
       <c r="D21" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="1" t="s">
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+    </row>
+    <row r="22" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="18" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="16" t="s">
@@ -1112,9 +1195,11 @@
       <c r="D22" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="5" t="s">
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+    </row>
+    <row r="23" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="19" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="14" t="s">
@@ -1126,9 +1211,11 @@
       <c r="D23" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="5" t="s">
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+    </row>
+    <row r="24" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="19" t="s">
         <v>28</v>
       </c>
       <c r="B24" s="14" t="s">
@@ -1140,9 +1227,11 @@
       <c r="D24" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="3" t="s">
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+    </row>
+    <row r="25" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="17" t="s">
         <v>29</v>
       </c>
       <c r="B25" s="15" t="s">
@@ -1154,9 +1243,11 @@
       <c r="D25" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="3" t="s">
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+    </row>
+    <row r="26" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="17" t="s">
         <v>30</v>
       </c>
       <c r="B26" s="15" t="s">
@@ -1168,9 +1259,11 @@
       <c r="D26" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="7" t="s">
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+    </row>
+    <row r="27" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="20" t="s">
         <v>27</v>
       </c>
       <c r="B27" s="8" t="s">
@@ -1182,26 +1275,34 @@
       <c r="D27" s="7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A28" s="7" t="s">
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+    </row>
+    <row r="28" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="23" t="s">
         <v>15</v>
       </c>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E29" s="24"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D28">
     <sortCondition ref="A1:A28"/>
   </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.11811023622047245" right="0.11811023622047245" top="0.15748031496062992" bottom="0.15748031496062992" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="87" fitToWidth="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>